<commit_message>
Hazard detection unit designed, and added to overall design. Muxes and fwds have also been added and the stalling of IF and ID have also been implemented to allow certain scenarios to stall. Have not yet thrown the Design through a test bench so im unsure if it works correctly or what the bugs are. New Design unit is called HazardDetectionUnit
</commit_message>
<xml_diff>
--- a/Project2/Lab Documents/ConsumerAndProducers.xlsx
+++ b/Project2/Lab Documents/ConsumerAndProducers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CPRE381\ProjectGit\cpre_381\Project2\Lab Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2943C54B-D434-4601-BBFA-A6E81EEDE379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41460B0-84E8-488F-9F68-E24F85BFDB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10005" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1D806764-18E3-406B-B390-0E24848C4A93}"/>
+    <workbookView xWindow="38805" yWindow="-16515" windowWidth="29040" windowHeight="15720" xr2:uid="{1D806764-18E3-406B-B390-0E24848C4A93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="99">
   <si>
     <t>and</t>
   </si>
@@ -242,32 +242,104 @@
     <t>…</t>
   </si>
   <si>
-    <t>if  ID/EX RS out == EX/MEM  out Reg ADDr</t>
-  </si>
-  <si>
     <t>if  ID/EX RS out == MEM/WB out Reg dst ADDr</t>
   </si>
   <si>
     <t>if  ID/EX Rt out == EX/MEM  out Reg dst ADDr</t>
   </si>
   <si>
-    <t>if ID/EX RS out == EX/MEM  out Reg dst ADDr</t>
-  </si>
-  <si>
     <t>if  ID/EX Rt out == MEM/WB  out Reg dst ADDr</t>
   </si>
   <si>
     <t>ELSE</t>
   </si>
   <si>
-    <t xml:space="preserve">if  ID/EX RS out == EX/MEM  out </t>
+    <t>if ID/EX Rs out == EX/MEM  out Reg dst ADDr</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == EX/MEM  out Reg ADDr &amp; Opcode == 100011</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == EX/MEM  out Reg ADDr &amp; Opcode == 100000</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == EX/MEM  out Reg ADDr &amp; Opcode == 100100</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == EX/MEM  out Reg ADDr &amp; Opcode == 100001</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == EX/MEM  out Reg ADDr &amp; Opcode == 100101</t>
+  </si>
+  <si>
+    <t>Instruction Type</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>Arithmatic &amp; logic MEM</t>
+  </si>
+  <si>
+    <t>Arithmatic &amp; logic WB</t>
+  </si>
+  <si>
+    <t>LW MEM</t>
+  </si>
+  <si>
+    <t>LB MEM</t>
+  </si>
+  <si>
+    <t>LBU MEM</t>
+  </si>
+  <si>
+    <t>LH MEM</t>
+  </si>
+  <si>
+    <t>LH WB</t>
+  </si>
+  <si>
+    <t>LBU WB</t>
+  </si>
+  <si>
+    <t>LB WB</t>
+  </si>
+  <si>
+    <t>LW WB</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == MEM/WB  out Reg ADDr &amp; Opcode == 100011</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == MEM/WB  out Reg ADDr &amp; Opcode == 100000</t>
+  </si>
+  <si>
+    <t>Producer And Consumer Chart</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == MEM/WB  out Reg ADDr &amp; Opcode == 100100</t>
+  </si>
+  <si>
+    <t>if  ID/EX Rs out == MEM/WB  out Reg ADDr &amp; Opcode == 100001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +430,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,8 +476,18 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -453,8 +549,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
@@ -462,8 +573,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -484,38 +597,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -527,20 +612,95 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Bad 4" xfId="2" xr:uid="{55ABEA83-5265-47C2-BE83-32EA174D9B18}"/>
     <cellStyle name="Good 2" xfId="3" xr:uid="{0F4CFC27-3F18-4454-86E2-4A8687CFDFD3}"/>
+    <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Neutral 1" xfId="4" xr:uid="{E07E30DF-2710-4ACD-A647-33CFBAA155C9}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{31E2416B-B536-43C1-AEA6-1E0B8C9E9208}"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning 1" xfId="5" xr:uid="{D137AC0E-EBE0-4AB2-A102-F6FCA8E640C0}"/>
     <cellStyle name="Warning 3" xfId="6" xr:uid="{3B7211CC-261E-4E8C-AF88-FA32D4659CB0}"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -707,13 +867,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>638242</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>638243</xdr:colOff>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>19094</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -751,21 +911,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71507023-7188-4315-AEE9-C284EBD8B002}" name="Table2" displayName="Table2" ref="A1:J35" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A1:J35" xr:uid="{71507023-7188-4315-AEE9-C284EBD8B002}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71507023-7188-4315-AEE9-C284EBD8B002}" name="Table2" displayName="Table2" ref="A2:J36" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A2:J36" xr:uid="{71507023-7188-4315-AEE9-C284EBD8B002}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8C8C032E-3EDD-48F9-9C71-50538FA99E82}" name="Intruction" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="19" dataCellStyle="Neutral 1"/>
-    <tableColumn id="2" xr3:uid="{E182A84C-652C-401A-AAD9-94344F87A7C4}" name="Producer" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{A4C539AE-F116-47D2-9DA6-CE0B9A37DE14}" name="Signal Where Produced" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{FB1A665C-6893-46DB-98FF-A47D45B30F7E}" name="Stage Produced In / FWD From" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{8507EA89-E35B-4274-926F-C3EA333A6CC2}" name="Stages Can Be Forward From (Check Drawing For Letter Key)" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{F87371DE-CF27-4B0B-A01F-78947591DB5D}" name="Consumer" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{A9CE5768-0154-4EFE-91FB-48EF76B6630C}" name="Signal #1 Where Value Is Consumed" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{241240E3-38B8-4187-A36E-E7EC8F95C695}" name="Stage Consumed In #1" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{9BE453BA-5A6E-4B54-B78A-A85BBCAB8B5F}" name="Signal #1 Where Value Is Consumed2" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{0E018E14-0DD6-44F4-A39F-0FD4EA291733}" name="Stage Consumed In #2" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{8C8C032E-3EDD-48F9-9C71-50538FA99E82}" name="Intruction" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="25" dataCellStyle="Neutral 1"/>
+    <tableColumn id="2" xr3:uid="{E182A84C-652C-401A-AAD9-94344F87A7C4}" name="Producer" dataDxfId="22" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{A4C539AE-F116-47D2-9DA6-CE0B9A37DE14}" name="Signal Where Produced" dataDxfId="20" totalsRowDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{FB1A665C-6893-46DB-98FF-A47D45B30F7E}" name="Stage Produced In / FWD From" dataDxfId="18" totalsRowDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{8507EA89-E35B-4274-926F-C3EA333A6CC2}" name="Stages Can Be Forward From (Check Drawing For Letter Key)" dataDxfId="16" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{F87371DE-CF27-4B0B-A01F-78947591DB5D}" name="Consumer" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{A9CE5768-0154-4EFE-91FB-48EF76B6630C}" name="Signal #1 Where Value Is Consumed" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{241240E3-38B8-4187-A36E-E7EC8F95C695}" name="Stage Consumed In #1" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{9BE453BA-5A6E-4B54-B78A-A85BBCAB8B5F}" name="Signal #1 Where Value Is Consumed2" dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{0E018E14-0DD6-44F4-A39F-0FD4EA291733}" name="Stage Consumed In #2" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FC6B174A-6B4D-49F4-AE70-7387B821CF06}" name="Table1467" displayName="Table1467" ref="A42:E56" totalsRowShown="0" headerRowDxfId="2" dataDxfId="5">
+  <autoFilter ref="A42:E56" xr:uid="{FC6B174A-6B4D-49F4-AE70-7387B821CF06}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{76763CF6-2DC6-499A-8209-468D26941F2A}" name="Instruction Type" dataDxfId="1" dataCellStyle="Note"/>
+    <tableColumn id="2" xr3:uid="{5DEF2580-6014-44FC-92BC-6249A40073BA}" name="Equation" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{FD95AF81-3F6B-4B70-A5AA-9B5C1707D24A}" name="Forwarder 1"/>
+    <tableColumn id="4" xr3:uid="{A9988BD9-3D3E-4707-8F55-6A0951B6BA4B}" name="Forwarder 2" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4FBA4AAB-5817-4139-B694-7968508029B6}" name="ELSE" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1086,17 +1260,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F782760-FCF8-4086-AFB8-37734B921443}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D31" sqref="D31"/>
+      <selection pane="topRight" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="36.53125" customWidth="1"/>
+    <col min="1" max="1" width="31.46484375" customWidth="1"/>
+    <col min="2" max="2" width="46.53125" customWidth="1"/>
     <col min="3" max="3" width="25.19921875" customWidth="1"/>
     <col min="4" max="4" width="35.73046875" customWidth="1"/>
     <col min="5" max="5" width="47.33203125" customWidth="1"/>
@@ -1107,84 +1281,65 @@
     <col min="11" max="11" width="44.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E2" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A2" s="2" t="s">
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>60</v>
@@ -1199,18 +1354,18 @@
         <v>46</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1240,10 +1395,10 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1265,17 +1420,16 @@
         <v>46</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
+      <c r="A6" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>33</v>
@@ -1305,10 +1459,11 @@
         <v>46</v>
       </c>
       <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A7" s="3" t="s">
-        <v>1</v>
+      <c r="A7" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>33</v>
@@ -1332,16 +1487,16 @@
         <v>46</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A8" s="4" t="s">
-        <v>2</v>
+      <c r="A8" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>33</v>
@@ -1356,13 +1511,13 @@
         <v>60</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>36</v>
@@ -1373,29 +1528,29 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
+      <c r="A9" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>36</v>
@@ -1406,20 +1561,20 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A10" s="4" t="s">
-        <v>4</v>
+      <c r="A10" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>33</v>
@@ -1431,16 +1586,16 @@
         <v>46</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
+      <c r="A11" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>33</v>
@@ -1472,8 +1627,8 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
+      <c r="A12" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>33</v>
@@ -1497,16 +1652,16 @@
         <v>46</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
+      <c r="A13" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>33</v>
@@ -1530,16 +1685,16 @@
         <v>46</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A14" s="4" t="s">
-        <v>8</v>
+      <c r="A14" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>33</v>
@@ -1563,16 +1718,16 @@
         <v>46</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
+      <c r="A15" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>33</v>
@@ -1596,16 +1751,16 @@
         <v>46</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A16" s="4" t="s">
-        <v>10</v>
+      <c r="A16" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>33</v>
@@ -1629,16 +1784,16 @@
         <v>46</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
+      <c r="A17" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>33</v>
@@ -1656,7 +1811,7 @@
         <v>33</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>46</v>
@@ -1670,8 +1825,8 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A18" s="4" t="s">
-        <v>12</v>
+      <c r="A18" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>33</v>
@@ -1703,8 +1858,8 @@
       <c r="K18" s="7"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
+      <c r="A19" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>33</v>
@@ -1736,53 +1891,53 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="C21" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>33</v>
@@ -1794,16 +1949,16 @@
         <v>46</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A22" s="4" t="s">
-        <v>16</v>
+      <c r="A22" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>33</v>
@@ -1835,20 +1990,20 @@
       <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A23" s="3" t="s">
-        <v>17</v>
+      <c r="A23" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>33</v>
@@ -1868,8 +2023,8 @@
       <c r="K23" s="7"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A24" s="4" t="s">
-        <v>18</v>
+      <c r="A24" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>34</v>
@@ -1901,8 +2056,8 @@
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A25" s="3" t="s">
-        <v>19</v>
+      <c r="A25" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>34</v>
@@ -1917,136 +2072,136 @@
         <v>36</v>
       </c>
       <c r="F25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A26" s="4" t="s">
+      <c r="C26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E27" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A27" s="3" t="s">
+      <c r="G27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="C28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A28" s="4" t="s">
+      <c r="H28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="B29" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>33</v>
@@ -2066,20 +2221,20 @@
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A30" s="4" t="s">
-        <v>24</v>
+      <c r="A30" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F30" s="7" t="s">
         <v>33</v>
@@ -2099,20 +2254,20 @@
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A31" s="3" t="s">
-        <v>25</v>
+      <c r="A31" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="11" t="s">
-        <v>54</v>
+      <c r="C31" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F31" s="7" t="s">
         <v>33</v>
@@ -2132,20 +2287,20 @@
       <c r="K31" s="7"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A32" s="4" t="s">
-        <v>26</v>
+      <c r="A32" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="7" t="s">
-        <v>35</v>
+      <c r="C32" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>33</v>
@@ -2157,15 +2312,16 @@
         <v>46</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>46</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="K32" s="7"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A33" s="3" t="s">
-        <v>27</v>
+      <c r="A33" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>33</v>
@@ -2196,8 +2352,8 @@
       </c>
     </row>
     <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A34" s="4" t="s">
-        <v>28</v>
+      <c r="A34" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>33</v>
@@ -2227,247 +2383,711 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="5" t="s">
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F35" s="7" t="s">
+      <c r="C36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J35" s="7" t="s">
+      <c r="G36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A40" s="17"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-    </row>
-    <row r="38" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="1"/>
-      <c r="B38" s="13" t="s">
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="26"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="6" t="s">
+      <c r="C42" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="D42" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="E42" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A43" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="14">
+        <v>101</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A44" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="14">
+        <v>101</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A45" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="14"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A46" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="14">
+        <v>100</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A47" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A39" s="16"/>
-      <c r="B39" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="7">
-        <v>101</v>
-      </c>
-      <c r="E39" s="7" t="s">
+      <c r="C47" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A40" s="17"/>
-      <c r="B40" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="7" t="s">
+      <c r="E47" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="14"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A48" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E40" s="10">
-        <v>101</v>
-      </c>
-      <c r="F40" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A41" s="18"/>
-      <c r="B41" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="7">
-        <v>100</v>
-      </c>
-      <c r="E41" s="7" t="s">
+      <c r="E48" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A49" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A42" s="17"/>
-      <c r="B42" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="7" t="s">
+      <c r="E49" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A50" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="7">
-        <v>100</v>
-      </c>
-      <c r="F42" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A43" s="18"/>
-      <c r="B43" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A44" s="17"/>
-      <c r="B44" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A45" s="18"/>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A46" s="17"/>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A47" s="18"/>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A48" s="17"/>
-    </row>
-    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A49" s="18"/>
-    </row>
-    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A50" s="17"/>
-    </row>
-    <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A51" s="18"/>
-    </row>
-    <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A52" s="17"/>
-    </row>
-    <row r="53" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A53" s="18"/>
-    </row>
-    <row r="54" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A54" s="17"/>
-    </row>
-    <row r="55" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A55" s="18"/>
-    </row>
-    <row r="56" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A56" s="17"/>
-    </row>
-    <row r="57" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A57" s="18"/>
-    </row>
-    <row r="58" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A58" s="17"/>
-    </row>
-    <row r="59" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A59" s="18"/>
-    </row>
-    <row r="60" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A60" s="17"/>
-    </row>
-    <row r="61" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A61" s="18"/>
-    </row>
-    <row r="62" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A62" s="17"/>
-    </row>
-    <row r="63" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A63" s="18"/>
-    </row>
-    <row r="64" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A64" s="17"/>
-    </row>
-    <row r="65" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A65" s="18"/>
-    </row>
-    <row r="66" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A66" s="17"/>
-    </row>
-    <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A67" s="18"/>
-    </row>
-    <row r="68" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A68" s="17"/>
-    </row>
-    <row r="69" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A69" s="18"/>
-    </row>
-    <row r="70" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A70" s="17"/>
-    </row>
-    <row r="71" spans="1:1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A71" s="18"/>
-    </row>
-    <row r="72" spans="1:1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="19"/>
+      <c r="E50" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A51" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="14"/>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A52" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="14"/>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A53" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="14"/>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A54" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="14"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A55" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A56" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" s="14"/>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A57" s="22"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A58" s="22"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A59" s="22"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A60" s="22"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A61" s="22"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A62" s="22"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A63" s="22"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A64" s="22"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A65" s="22"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A66" s="22"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A67" s="23"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A68" s="23"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A69" s="22"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A70" s="22"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A71" s="23"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A72" s="23"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A73" s="22"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A74" s="22"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="7"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A75" s="22"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A76" s="22"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="7"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A87" s="16"/>
+      <c r="B87" s="16"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="16"/>
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="15"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="15"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A90" s="17"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+    </row>
+    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A91" s="22"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+    </row>
+    <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A92" s="22"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A93" s="22"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+    </row>
+    <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A94" s="22"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+    </row>
+    <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A95" s="22"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+    </row>
+    <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A96" s="22"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+    </row>
+    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A97" s="23"/>
+      <c r="B97" s="20"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+    </row>
+    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A98" s="23"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+    </row>
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A99" s="22"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
+    </row>
+    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A100" s="22"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+    </row>
+    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A101" s="23"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+    </row>
+    <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A102" s="23"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+    </row>
+    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A103" s="22"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+    </row>
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A104" s="22"/>
+      <c r="B104" s="12"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A105" s="22"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+    </row>
+    <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A106" s="22"/>
+      <c r="B106" s="12"/>
+      <c r="C106" s="6"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
+  <mergeCells count="4">
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A87:F87"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A41:E41"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Im crying alot today for some reason
</commit_message>
<xml_diff>
--- a/Project2/Lab Documents/ConsumerAndProducers.xlsx
+++ b/Project2/Lab Documents/ConsumerAndProducers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CPRE381\ProjectGit\cpre_381\Project2\Lab Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8d6d17d704a0d79/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41460B0-84E8-488F-9F68-E24F85BFDB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{61F5ED55-97A8-497F-B9FB-6C30F900A785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23EF04B2-D1D6-48AB-A8E3-E7CFD9382007}"/>
   <bookViews>
-    <workbookView xWindow="38805" yWindow="-16515" windowWidth="29040" windowHeight="15720" xr2:uid="{1D806764-18E3-406B-B390-0E24848C4A93}"/>
+    <workbookView xWindow="10005" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{1D806764-18E3-406B-B390-0E24848C4A93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="109">
   <si>
     <t>and</t>
   </si>
@@ -287,12 +287,6 @@
     <t>011</t>
   </si>
   <si>
-    <t>Arithmatic &amp; logic MEM</t>
-  </si>
-  <si>
-    <t>Arithmatic &amp; logic WB</t>
-  </si>
-  <si>
     <t>LW MEM</t>
   </si>
   <si>
@@ -333,13 +327,49 @@
   </si>
   <si>
     <t>if  ID/EX Rs out == MEM/WB  out Reg ADDr &amp; Opcode == 100001</t>
+  </si>
+  <si>
+    <t>Arithmatic &amp; logic MEM #1</t>
+  </si>
+  <si>
+    <t>Arithmatic &amp; logic MEM #2</t>
+  </si>
+  <si>
+    <t>Arithmatic &amp; logic WB #3</t>
+  </si>
+  <si>
+    <t>Arithmatic &amp; logic WB #4</t>
+  </si>
+  <si>
+    <t>LHU MEM</t>
+  </si>
+  <si>
+    <t>LHU WB</t>
+  </si>
+  <si>
+    <t>Stall When</t>
+  </si>
+  <si>
+    <t>Stall</t>
+  </si>
+  <si>
+    <t>if(WB WE == 1 &amp; rt |rs  != dst</t>
+  </si>
+  <si>
+    <t>if ((i_EX_Reg_Rt = "00000") or i_EX_Reg_Rt = "00000")</t>
+  </si>
+  <si>
+    <t>Catch bad fwd</t>
+  </si>
+  <si>
+    <t>Catch Back To Back write to same reg but fwd not needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,6 +474,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -487,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -564,6 +613,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -576,7 +638,7 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -626,13 +688,7 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -641,13 +697,31 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="6" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="14" fillId="6" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="7" borderId="6" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Bad 4" xfId="2" xr:uid="{55ABEA83-5265-47C2-BE83-32EA174D9B18}"/>
@@ -661,6 +735,14 @@
     <cellStyle name="Warning 3" xfId="6" xr:uid="{3B7211CC-261E-4E8C-AF88-FA32D4659CB0}"/>
   </cellStyles>
   <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -687,18 +769,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -772,6 +846,13 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -780,12 +861,8 @@
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -806,13 +883,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="medium">
@@ -821,8 +891,12 @@
         <right style="thin">
           <color auto="1"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -914,30 +988,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{71507023-7188-4315-AEE9-C284EBD8B002}" name="Table2" displayName="Table2" ref="A2:J36" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A2:J36" xr:uid="{71507023-7188-4315-AEE9-C284EBD8B002}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8C8C032E-3EDD-48F9-9C71-50538FA99E82}" name="Intruction" totalsRowLabel="Total" dataDxfId="24" totalsRowDxfId="25" dataCellStyle="Neutral 1"/>
-    <tableColumn id="2" xr3:uid="{E182A84C-652C-401A-AAD9-94344F87A7C4}" name="Producer" dataDxfId="22" totalsRowDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{A4C539AE-F116-47D2-9DA6-CE0B9A37DE14}" name="Signal Where Produced" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{FB1A665C-6893-46DB-98FF-A47D45B30F7E}" name="Stage Produced In / FWD From" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{8507EA89-E35B-4274-926F-C3EA333A6CC2}" name="Stages Can Be Forward From (Check Drawing For Letter Key)" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{F87371DE-CF27-4B0B-A01F-78947591DB5D}" name="Consumer" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{A9CE5768-0154-4EFE-91FB-48EF76B6630C}" name="Signal #1 Where Value Is Consumed" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{241240E3-38B8-4187-A36E-E7EC8F95C695}" name="Stage Consumed In #1" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{9BE453BA-5A6E-4B54-B78A-A85BBCAB8B5F}" name="Signal #1 Where Value Is Consumed2" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{0E018E14-0DD6-44F4-A39F-0FD4EA291733}" name="Stage Consumed In #2" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{8C8C032E-3EDD-48F9-9C71-50538FA99E82}" name="Intruction" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24" dataCellStyle="Neutral 1"/>
+    <tableColumn id="2" xr3:uid="{E182A84C-652C-401A-AAD9-94344F87A7C4}" name="Producer" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{A4C539AE-F116-47D2-9DA6-CE0B9A37DE14}" name="Signal Where Produced" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{FB1A665C-6893-46DB-98FF-A47D45B30F7E}" name="Stage Produced In / FWD From" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{8507EA89-E35B-4274-926F-C3EA333A6CC2}" name="Stages Can Be Forward From (Check Drawing For Letter Key)" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{F87371DE-CF27-4B0B-A01F-78947591DB5D}" name="Consumer" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{A9CE5768-0154-4EFE-91FB-48EF76B6630C}" name="Signal #1 Where Value Is Consumed" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{241240E3-38B8-4187-A36E-E7EC8F95C695}" name="Stage Consumed In #1" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{9BE453BA-5A6E-4B54-B78A-A85BBCAB8B5F}" name="Signal #1 Where Value Is Consumed2" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{0E018E14-0DD6-44F4-A39F-0FD4EA291733}" name="Stage Consumed In #2" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FC6B174A-6B4D-49F4-AE70-7387B821CF06}" name="Table1467" displayName="Table1467" ref="A42:E56" totalsRowShown="0" headerRowDxfId="2" dataDxfId="5">
-  <autoFilter ref="A42:E56" xr:uid="{FC6B174A-6B4D-49F4-AE70-7387B821CF06}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FC6B174A-6B4D-49F4-AE70-7387B821CF06}" name="Table1467" displayName="Table1467" ref="A42:E59" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A42:E59" xr:uid="{FC6B174A-6B4D-49F4-AE70-7387B821CF06}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{76763CF6-2DC6-499A-8209-468D26941F2A}" name="Instruction Type" dataDxfId="1" dataCellStyle="Note"/>
-    <tableColumn id="2" xr3:uid="{5DEF2580-6014-44FC-92BC-6249A40073BA}" name="Equation" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{76763CF6-2DC6-499A-8209-468D26941F2A}" name="Instruction Type" dataDxfId="3" dataCellStyle="Note"/>
+    <tableColumn id="2" xr3:uid="{5DEF2580-6014-44FC-92BC-6249A40073BA}" name="Equation" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{FD95AF81-3F6B-4B70-A5AA-9B5C1707D24A}" name="Forwarder 1"/>
-    <tableColumn id="4" xr3:uid="{A9988BD9-3D3E-4707-8F55-6A0951B6BA4B}" name="Forwarder 2" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4FBA4AAB-5817-4139-B694-7968508029B6}" name="ELSE" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A9988BD9-3D3E-4707-8F55-6A0951B6BA4B}" name="Forwarder 2" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{4FBA4AAB-5817-4139-B694-7968508029B6}" name="ELSE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1262,14 +1336,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F782760-FCF8-4086-AFB8-37734B921443}">
   <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E49" sqref="E49"/>
+      <selection pane="topRight" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.46484375" customWidth="1"/>
+    <col min="1" max="1" width="42.53125" customWidth="1"/>
     <col min="2" max="2" width="46.53125" customWidth="1"/>
     <col min="3" max="3" width="25.19921875" customWidth="1"/>
     <col min="4" max="4" width="35.73046875" customWidth="1"/>
@@ -1282,18 +1356,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="A1" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="6" t="s">
@@ -2448,25 +2522,25 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A37" s="16"/>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A38" s="19"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
@@ -2482,23 +2556,23 @@
       <c r="F40" s="13"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A41" s="24" t="s">
+      <c r="A41" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="26"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="16" t="s">
         <v>65</v>
       </c>
       <c r="D42" s="14" t="s">
@@ -2510,82 +2584,82 @@
       <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="13">
+        <v>101</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="15"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A44" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="13">
+        <v>101</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A45" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="14"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A46" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="24">
+        <v>100</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F46" s="14"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A47" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="14">
-        <v>101</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F43" s="15"/>
-    </row>
-    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A44" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="14">
-        <v>101</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F44" s="13"/>
-    </row>
-    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A45" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F45" s="14"/>
-    </row>
-    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A46" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D46" s="14">
-        <v>100</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F46" s="14"/>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A47" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>73</v>
       </c>
       <c r="C47" s="14" t="s">
@@ -2600,14 +2674,14 @@
       <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="20" t="s">
-        <v>94</v>
-      </c>
       <c r="C48" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D48" s="14" t="s">
         <v>67</v>
@@ -2618,10 +2692,10 @@
       <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A49" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="20" t="s">
+      <c r="A49" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="19" t="s">
         <v>74</v>
       </c>
       <c r="C49" s="14" t="s">
@@ -2636,14 +2710,14 @@
       <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A50" s="23" t="s">
+      <c r="A50" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="14" t="s">
         <v>91</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>93</v>
       </c>
       <c r="D50" s="14" t="s">
         <v>67</v>
@@ -2654,10 +2728,10 @@
       <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A51" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="B51" s="20" t="s">
+      <c r="A51" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="19" t="s">
         <v>75</v>
       </c>
       <c r="C51" s="14" t="s">
@@ -2672,14 +2746,14 @@
       <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A52" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>97</v>
+      <c r="A52" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>95</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D52" s="14" t="s">
         <v>67</v>
@@ -2690,10 +2764,10 @@
       <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A53" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="20" t="s">
+      <c r="A53" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="19" t="s">
         <v>76</v>
       </c>
       <c r="C53" s="14" t="s">
@@ -2708,14 +2782,14 @@
       <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A54" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>98</v>
+      <c r="A54" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D54" s="14" t="s">
         <v>67</v>
@@ -2726,10 +2800,10 @@
       <c r="F54" s="14"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A55" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="20" t="s">
+      <c r="A55" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="19" t="s">
         <v>77</v>
       </c>
       <c r="C55" s="14" t="s">
@@ -2744,14 +2818,14 @@
       <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A56" s="23" t="s">
-        <v>89</v>
+      <c r="A56" s="21" t="s">
+        <v>102</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>77</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D56" s="7" t="s">
         <v>67</v>
@@ -2762,36 +2836,67 @@
       <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A57" s="22"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="A57" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A58" s="22"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="7"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A59" s="22"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
+      <c r="A58" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>67</v>
+      </c>
       <c r="F59" s="14"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A60" s="22"/>
+      <c r="A60" s="20"/>
       <c r="B60" s="12"/>
       <c r="C60" s="6"/>
       <c r="D60" s="14"/>
       <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A61" s="22"/>
+      <c r="A61" s="20"/>
       <c r="B61" s="18"/>
       <c r="C61" s="13"/>
       <c r="D61" s="14"/>
@@ -2799,7 +2904,7 @@
       <c r="F61" s="14"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A62" s="22"/>
+      <c r="A62" s="20"/>
       <c r="B62" s="18"/>
       <c r="C62" s="13"/>
       <c r="D62" s="14"/>
@@ -2807,23 +2912,23 @@
       <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A63" s="22"/>
-      <c r="B63" s="20"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="19"/>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A64" s="22"/>
-      <c r="B64" s="20"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A65" s="22"/>
+      <c r="A65" s="20"/>
       <c r="B65" s="18"/>
       <c r="C65" s="13"/>
       <c r="D65" s="14"/>
@@ -2831,7 +2936,7 @@
       <c r="F65" s="14"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A66" s="22"/>
+      <c r="A66" s="20"/>
       <c r="B66" s="18"/>
       <c r="C66" s="13"/>
       <c r="D66" s="14"/>
@@ -2839,23 +2944,23 @@
       <c r="F66" s="14"/>
     </row>
     <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A67" s="23"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="21"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A68" s="23"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
     </row>
     <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A69" s="22"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="18"/>
       <c r="C69" s="13"/>
       <c r="D69" s="14"/>
@@ -2863,7 +2968,7 @@
       <c r="F69" s="14"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A70" s="22"/>
+      <c r="A70" s="20"/>
       <c r="B70" s="18"/>
       <c r="C70" s="13"/>
       <c r="D70" s="14"/>
@@ -2871,23 +2976,23 @@
       <c r="F70" s="14"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A71" s="23"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="21"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
     </row>
     <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A72" s="23"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="21"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
     </row>
     <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A73" s="22"/>
+      <c r="A73" s="20"/>
       <c r="B73" s="18"/>
       <c r="C73" s="13"/>
       <c r="D73" s="14"/>
@@ -2895,14 +3000,14 @@
       <c r="F73" s="14"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A74" s="22"/>
+      <c r="A74" s="20"/>
       <c r="B74" s="12"/>
       <c r="C74" s="6"/>
       <c r="D74" s="14"/>
       <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A75" s="22"/>
+      <c r="A75" s="20"/>
       <c r="B75" s="18"/>
       <c r="C75" s="13"/>
       <c r="D75" s="14"/>
@@ -2910,32 +3015,32 @@
       <c r="F75" s="14"/>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A76" s="22"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="12"/>
       <c r="C76" s="6"/>
       <c r="D76" s="14"/>
       <c r="E76" s="7"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A87" s="16"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="16"/>
-      <c r="D87" s="16"/>
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
+      <c r="A87" s="26"/>
+      <c r="B87" s="26"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="26"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A88" s="19"/>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
+      <c r="A88" s="16"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
       <c r="D88" s="15"/>
       <c r="E88" s="15"/>
       <c r="F88" s="15"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A89" s="19"/>
-      <c r="B89" s="19"/>
-      <c r="C89" s="19"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="C89" s="16"/>
       <c r="D89" s="15"/>
       <c r="E89" s="15"/>
       <c r="F89" s="15"/>
@@ -2949,7 +3054,7 @@
       <c r="F90" s="13"/>
     </row>
     <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A91" s="22"/>
+      <c r="A91" s="20"/>
       <c r="B91" s="18"/>
       <c r="C91" s="13"/>
       <c r="D91" s="14"/>
@@ -2957,7 +3062,7 @@
       <c r="F91" s="14"/>
     </row>
     <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A92" s="22"/>
+      <c r="A92" s="20"/>
       <c r="B92" s="18"/>
       <c r="C92" s="13"/>
       <c r="D92" s="14"/>
@@ -2965,23 +3070,23 @@
       <c r="F92" s="14"/>
     </row>
     <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A93" s="22"/>
-      <c r="B93" s="20"/>
+      <c r="A93" s="20"/>
+      <c r="B93" s="19"/>
       <c r="C93" s="14"/>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="14"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A94" s="22"/>
-      <c r="B94" s="20"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="19"/>
       <c r="C94" s="14"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="14"/>
     </row>
     <row r="95" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A95" s="22"/>
+      <c r="A95" s="20"/>
       <c r="B95" s="18"/>
       <c r="C95" s="13"/>
       <c r="D95" s="14"/>
@@ -2989,7 +3094,7 @@
       <c r="F95" s="14"/>
     </row>
     <row r="96" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A96" s="22"/>
+      <c r="A96" s="20"/>
       <c r="B96" s="18"/>
       <c r="C96" s="13"/>
       <c r="D96" s="14"/>
@@ -2997,23 +3102,23 @@
       <c r="F96" s="14"/>
     </row>
     <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A97" s="23"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="21"/>
+      <c r="A97" s="21"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="14"/>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="14"/>
     </row>
     <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A98" s="23"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="21"/>
+      <c r="A98" s="21"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="14"/>
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="14"/>
     </row>
     <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A99" s="22"/>
+      <c r="A99" s="20"/>
       <c r="B99" s="18"/>
       <c r="C99" s="13"/>
       <c r="D99" s="14"/>
@@ -3021,7 +3126,7 @@
       <c r="F99" s="14"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A100" s="22"/>
+      <c r="A100" s="20"/>
       <c r="B100" s="18"/>
       <c r="C100" s="13"/>
       <c r="D100" s="14"/>
@@ -3029,23 +3134,23 @@
       <c r="F100" s="14"/>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A101" s="23"/>
-      <c r="B101" s="20"/>
-      <c r="C101" s="21"/>
+      <c r="A101" s="21"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="14"/>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
       <c r="F101" s="14"/>
     </row>
     <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A102" s="23"/>
-      <c r="B102" s="20"/>
-      <c r="C102" s="21"/>
+      <c r="A102" s="21"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="14"/>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="14"/>
     </row>
     <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A103" s="22"/>
+      <c r="A103" s="20"/>
       <c r="B103" s="18"/>
       <c r="C103" s="13"/>
       <c r="D103" s="14"/>
@@ -3053,14 +3158,14 @@
       <c r="F103" s="14"/>
     </row>
     <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A104" s="22"/>
+      <c r="A104" s="20"/>
       <c r="B104" s="12"/>
       <c r="C104" s="6"/>
       <c r="D104" s="14"/>
       <c r="E104" s="7"/>
     </row>
     <row r="105" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A105" s="22"/>
+      <c r="A105" s="20"/>
       <c r="B105" s="18"/>
       <c r="C105" s="13"/>
       <c r="D105" s="14"/>
@@ -3068,7 +3173,7 @@
       <c r="F105" s="14"/>
     </row>
     <row r="106" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A106" s="22"/>
+      <c r="A106" s="20"/>
       <c r="B106" s="12"/>
       <c r="C106" s="6"/>
       <c r="D106" s="14"/>

</xml_diff>